<commit_message>
Added Mid-Project Progress Report and Updated Gantt chart
</commit_message>
<xml_diff>
--- a/ZackRileyGanttChart.xlsx
+++ b/ZackRileyGanttChart.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{067686A0-371C-402C-82CB-8B7723D967AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39356920-8D27-4576-B0F2-A3FD781B8F77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="17115" windowHeight="11475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -932,6 +932,18 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="12">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="9">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
       <alignment horizontal="right" indent="1"/>
     </xf>
@@ -939,18 +951,6 @@
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="9">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Comma" xfId="4" builtinId="3" customBuiltin="1"/>
@@ -1520,8 +1520,8 @@
   <dimension ref="A1:BL36"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D27" sqref="D27"/>
+      <pane ySplit="6" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -1568,14 +1568,14 @@
       <c r="B3" s="65" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="85" t="s">
+      <c r="C3" s="89" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="86"/>
-      <c r="E3" s="91">
+      <c r="D3" s="90"/>
+      <c r="E3" s="88">
         <v>44487</v>
       </c>
-      <c r="F3" s="91"/>
+      <c r="F3" s="88"/>
     </row>
     <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="59" t="s">
@@ -1584,104 +1584,104 @@
       <c r="B4" s="65" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="85" t="s">
+      <c r="C4" s="89" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="86"/>
+      <c r="D4" s="90"/>
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="88">
+      <c r="I4" s="85">
         <f>I5</f>
         <v>44487</v>
       </c>
-      <c r="J4" s="89"/>
-      <c r="K4" s="89"/>
-      <c r="L4" s="89"/>
-      <c r="M4" s="89"/>
-      <c r="N4" s="89"/>
-      <c r="O4" s="90"/>
-      <c r="P4" s="88">
+      <c r="J4" s="86"/>
+      <c r="K4" s="86"/>
+      <c r="L4" s="86"/>
+      <c r="M4" s="86"/>
+      <c r="N4" s="86"/>
+      <c r="O4" s="87"/>
+      <c r="P4" s="85">
         <f>P5</f>
         <v>44494</v>
       </c>
-      <c r="Q4" s="89"/>
-      <c r="R4" s="89"/>
-      <c r="S4" s="89"/>
-      <c r="T4" s="89"/>
-      <c r="U4" s="89"/>
-      <c r="V4" s="90"/>
-      <c r="W4" s="88">
+      <c r="Q4" s="86"/>
+      <c r="R4" s="86"/>
+      <c r="S4" s="86"/>
+      <c r="T4" s="86"/>
+      <c r="U4" s="86"/>
+      <c r="V4" s="87"/>
+      <c r="W4" s="85">
         <f>W5</f>
         <v>44501</v>
       </c>
-      <c r="X4" s="89"/>
-      <c r="Y4" s="89"/>
-      <c r="Z4" s="89"/>
-      <c r="AA4" s="89"/>
-      <c r="AB4" s="89"/>
-      <c r="AC4" s="90"/>
-      <c r="AD4" s="88">
+      <c r="X4" s="86"/>
+      <c r="Y4" s="86"/>
+      <c r="Z4" s="86"/>
+      <c r="AA4" s="86"/>
+      <c r="AB4" s="86"/>
+      <c r="AC4" s="87"/>
+      <c r="AD4" s="85">
         <f>AD5</f>
         <v>44508</v>
       </c>
-      <c r="AE4" s="89"/>
-      <c r="AF4" s="89"/>
-      <c r="AG4" s="89"/>
-      <c r="AH4" s="89"/>
-      <c r="AI4" s="89"/>
-      <c r="AJ4" s="90"/>
-      <c r="AK4" s="88">
+      <c r="AE4" s="86"/>
+      <c r="AF4" s="86"/>
+      <c r="AG4" s="86"/>
+      <c r="AH4" s="86"/>
+      <c r="AI4" s="86"/>
+      <c r="AJ4" s="87"/>
+      <c r="AK4" s="85">
         <f>AK5</f>
         <v>44515</v>
       </c>
-      <c r="AL4" s="89"/>
-      <c r="AM4" s="89"/>
-      <c r="AN4" s="89"/>
-      <c r="AO4" s="89"/>
-      <c r="AP4" s="89"/>
-      <c r="AQ4" s="90"/>
-      <c r="AR4" s="88">
+      <c r="AL4" s="86"/>
+      <c r="AM4" s="86"/>
+      <c r="AN4" s="86"/>
+      <c r="AO4" s="86"/>
+      <c r="AP4" s="86"/>
+      <c r="AQ4" s="87"/>
+      <c r="AR4" s="85">
         <f>AR5</f>
         <v>44522</v>
       </c>
-      <c r="AS4" s="89"/>
-      <c r="AT4" s="89"/>
-      <c r="AU4" s="89"/>
-      <c r="AV4" s="89"/>
-      <c r="AW4" s="89"/>
-      <c r="AX4" s="90"/>
-      <c r="AY4" s="88">
+      <c r="AS4" s="86"/>
+      <c r="AT4" s="86"/>
+      <c r="AU4" s="86"/>
+      <c r="AV4" s="86"/>
+      <c r="AW4" s="86"/>
+      <c r="AX4" s="87"/>
+      <c r="AY4" s="85">
         <f>AY5</f>
         <v>44529</v>
       </c>
-      <c r="AZ4" s="89"/>
-      <c r="BA4" s="89"/>
-      <c r="BB4" s="89"/>
-      <c r="BC4" s="89"/>
-      <c r="BD4" s="89"/>
-      <c r="BE4" s="90"/>
-      <c r="BF4" s="88">
+      <c r="AZ4" s="86"/>
+      <c r="BA4" s="86"/>
+      <c r="BB4" s="86"/>
+      <c r="BC4" s="86"/>
+      <c r="BD4" s="86"/>
+      <c r="BE4" s="87"/>
+      <c r="BF4" s="85">
         <f>BF5</f>
         <v>44536</v>
       </c>
-      <c r="BG4" s="89"/>
-      <c r="BH4" s="89"/>
-      <c r="BI4" s="89"/>
-      <c r="BJ4" s="89"/>
-      <c r="BK4" s="89"/>
-      <c r="BL4" s="90"/>
+      <c r="BG4" s="86"/>
+      <c r="BH4" s="86"/>
+      <c r="BI4" s="86"/>
+      <c r="BJ4" s="86"/>
+      <c r="BK4" s="86"/>
+      <c r="BL4" s="87"/>
     </row>
     <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="59" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="87"/>
-      <c r="C5" s="87"/>
-      <c r="D5" s="87"/>
-      <c r="E5" s="87"/>
-      <c r="F5" s="87"/>
-      <c r="G5" s="87"/>
+      <c r="B5" s="91"/>
+      <c r="C5" s="91"/>
+      <c r="D5" s="91"/>
+      <c r="E5" s="91"/>
+      <c r="F5" s="91"/>
+      <c r="G5" s="91"/>
       <c r="I5" s="11">
         <f>Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
         <v>44487</v>
@@ -3586,12 +3586,12 @@
         <v>0</v>
       </c>
       <c r="E25" s="68">
-        <f>E23</f>
-        <v>44497</v>
+        <f>E24</f>
+        <v>44503</v>
       </c>
       <c r="F25" s="68">
         <f>E25+4</f>
-        <v>44501</v>
+        <v>44507</v>
       </c>
       <c r="G25" s="17"/>
       <c r="H25" s="17">
@@ -3736,7 +3736,9 @@
       <c r="C27" s="78" t="s">
         <v>42</v>
       </c>
-      <c r="D27" s="37"/>
+      <c r="D27" s="37">
+        <v>0.9</v>
+      </c>
       <c r="E27" s="69">
         <v>44501</v>
       </c>
@@ -3813,7 +3815,9 @@
       <c r="C28" s="78" t="s">
         <v>42</v>
       </c>
-      <c r="D28" s="37"/>
+      <c r="D28" s="37">
+        <v>0</v>
+      </c>
       <c r="E28" s="69">
         <v>44530</v>
       </c>
@@ -4251,6 +4255,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="E3:F3"/>
@@ -4258,11 +4267,6 @@
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D33">
     <cfRule type="dataBar" priority="14">

</xml_diff>